<commit_message>
master: Increased angle after wave 10, up to 70
</commit_message>
<xml_diff>
--- a/Balance.xlsx
+++ b/Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\workspace\LD56\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3A8827-D146-4ED6-9D7C-41F3E6665D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715BD071-DF99-415D-978E-E3DA18D56782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,13 +116,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,31 +406,31 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
     <col min="16" max="16" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
@@ -439,7 +439,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="3"/>
+      <c r="F2" s="2"/>
       <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
@@ -481,7 +481,7 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I3">
@@ -503,7 +503,7 @@
         <v>20</v>
       </c>
       <c r="O3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P3">
         <f>(K3+(3*L3)+(2*M3))*J3</f>
@@ -526,7 +526,7 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <f>(1/B4)*D4*C4*E4</f>
         <v>3.3333333333333335</v>
       </c>
@@ -549,7 +549,7 @@
         <v>20</v>
       </c>
       <c r="O4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P8" si="0">(K4+(3*L4)+(2*M4))*J4</f>
@@ -569,7 +569,7 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <f t="shared" ref="F5:F19" si="1">(1/B5)*D5*C5*E5</f>
         <v>6.666666666666667</v>
       </c>
@@ -592,7 +592,7 @@
         <v>20</v>
       </c>
       <c r="O5">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
@@ -612,7 +612,7 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -635,7 +635,7 @@
         <v>20</v>
       </c>
       <c r="O6">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
@@ -655,7 +655,7 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <f t="shared" si="1"/>
         <v>13.333333333333334</v>
       </c>
@@ -678,7 +678,7 @@
         <v>20</v>
       </c>
       <c r="O7">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
@@ -698,7 +698,7 @@
       <c r="E8">
         <v>1.3</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
         <v>4.3333333333333339</v>
       </c>
@@ -722,7 +722,7 @@
         <v>22</v>
       </c>
       <c r="O8">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
@@ -742,7 +742,7 @@
       <c r="E9">
         <v>1.3</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <f t="shared" si="1"/>
         <v>8.6666666666666679</v>
       </c>
@@ -766,7 +766,7 @@
         <v>24</v>
       </c>
       <c r="O9">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="P9">
         <f>(K9+(3*L9)+(2*M9))*J9</f>
@@ -786,7 +786,7 @@
       <c r="E10">
         <v>1.3</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -810,7 +810,7 @@
         <v>26</v>
       </c>
       <c r="O10">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="P10">
         <f>(K10+(3*L10)+(2*M10))*J10</f>
@@ -830,7 +830,7 @@
       <c r="E11">
         <v>1.3</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <f t="shared" si="1"/>
         <v>17.333333333333336</v>
       </c>
@@ -854,7 +854,7 @@
         <v>28</v>
       </c>
       <c r="O11">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="P11">
         <f>(K11+(3*L11)+(2*M11))*J11</f>
@@ -874,7 +874,7 @@
       <c r="E12">
         <v>1.6</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <f t="shared" si="1"/>
         <v>5.3333333333333339</v>
       </c>
@@ -898,7 +898,7 @@
         <v>30</v>
       </c>
       <c r="O12">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="P12">
         <f t="shared" ref="P12" si="3">(K12+(3*L12)+(2*M12))*J12</f>
@@ -918,7 +918,7 @@
       <c r="E13">
         <v>1.6</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
         <v>10.666666666666668</v>
       </c>
@@ -951,7 +951,7 @@
       </c>
       <c r="O13">
         <f>O12+1</f>
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="P13">
         <f>(K13+(3*L13)+(2*M13))*J13</f>
@@ -971,7 +971,7 @@
       <c r="E14">
         <v>1.6</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="O14">
         <f t="shared" ref="O14:O24" si="8">O13+1</f>
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="P14">
         <f t="shared" ref="P14:P24" si="9">(K14+(3*L14)+(2*M14))*J14</f>
@@ -1021,7 +1021,7 @@
       <c r="E15">
         <v>1.6</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <f t="shared" si="1"/>
         <v>21.333333333333336</v>
       </c>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="O15">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="P15">
         <f t="shared" si="9"/>
@@ -1071,7 +1071,7 @@
       <c r="E16">
         <v>1.9</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <f t="shared" si="1"/>
         <v>6.333333333333333</v>
       </c>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="O16">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="P16">
         <f t="shared" si="9"/>
@@ -1121,7 +1121,7 @@
       <c r="E17">
         <v>1.9</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <f t="shared" si="1"/>
         <v>12.666666666666666</v>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="O17">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="P17">
         <f t="shared" si="9"/>
@@ -1171,7 +1171,7 @@
       <c r="E18">
         <v>1.9</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="O18">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="P18">
         <f t="shared" si="9"/>
@@ -1221,7 +1221,7 @@
       <c r="E19">
         <v>1.9</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <f t="shared" si="1"/>
         <v>25.333333333333332</v>
       </c>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="O19">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="P19">
         <f t="shared" si="9"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="O20">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="P20">
         <f t="shared" si="9"/>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="O21">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="P21">
         <f t="shared" si="9"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="O22">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="P22">
         <f t="shared" si="9"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="O23">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="P23">
         <f t="shared" si="9"/>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="O24">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="P24">
         <f t="shared" si="9"/>

</xml_diff>